<commit_message>
IR Circuit Test Code
I doubt this is very important
</commit_message>
<xml_diff>
--- a/Lab/Lab Report Tracking Sheet.xlsx
+++ b/Lab/Lab Report Tracking Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Black Rod</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>Not Nessisary</t>
-  </si>
-  <si>
-    <t>**** To avoid fuckups, each time you update this table, make a new sheet. Label it with you name and time/date. This should help us stay organized.</t>
   </si>
 </sst>
 </file>
@@ -472,7 +469,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,9 +612,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="A11" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>